<commit_message>
added two more bet buttons, change the positions of the buttons
</commit_message>
<xml_diff>
--- a/Assets/images/prereq/datsa.xlsx
+++ b/Assets/images/prereq/datsa.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>bet100</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>Result</t>
+  </si>
+  <si>
+    <t>bet25</t>
+  </si>
+  <si>
+    <t>bet50</t>
   </si>
 </sst>
 </file>
@@ -392,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,16 +425,16 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C2">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D2">
-        <v>228</v>
+        <v>178</v>
       </c>
       <c r="E2">
-        <v>224</v>
+        <v>307</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -436,123 +442,123 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C3">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D3">
-        <v>294</v>
+        <v>237</v>
       </c>
       <c r="E3">
-        <v>224</v>
+        <v>307</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="B4">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C4">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D4">
-        <v>360</v>
+        <v>298</v>
       </c>
       <c r="E4">
-        <v>224</v>
+        <v>307</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B5">
-        <v>116</v>
+        <v>48</v>
       </c>
       <c r="C5">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="D5">
-        <v>260</v>
+        <v>357</v>
       </c>
       <c r="E5">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B6">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C6">
         <v>48</v>
       </c>
       <c r="D6">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="E6">
-        <v>15</v>
+        <v>307</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B7">
-        <v>47</v>
+        <v>131</v>
       </c>
       <c r="C7">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="D7">
-        <v>182</v>
+        <v>265</v>
       </c>
       <c r="E7">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>46</v>
+      </c>
+      <c r="C8">
+        <v>48</v>
+      </c>
+      <c r="D8">
+        <v>413</v>
+      </c>
+      <c r="E8">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C9">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D9">
-        <v>243</v>
+        <v>182</v>
       </c>
       <c r="E9">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10">
-        <v>46</v>
-      </c>
-      <c r="C10">
-        <v>45</v>
-      </c>
-      <c r="D10">
-        <v>297</v>
-      </c>
-      <c r="E10">
-        <v>146</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>45</v>
@@ -561,61 +567,61 @@
         <v>45</v>
       </c>
       <c r="D11">
-        <v>352</v>
+        <v>243</v>
       </c>
       <c r="E11">
         <v>146</v>
       </c>
     </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>46</v>
+      </c>
+      <c r="C12">
+        <v>45</v>
+      </c>
+      <c r="D12">
+        <v>297</v>
+      </c>
+      <c r="E12">
+        <v>146</v>
+      </c>
+    </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>45</v>
+      </c>
+      <c r="C13">
+        <v>45</v>
+      </c>
       <c r="D13">
-        <f>D10-D9</f>
+        <v>352</v>
+      </c>
+      <c r="E13">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <f>D12-D11</f>
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D14">
-        <f>D11-D10</f>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <f>D13-D12</f>
         <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16">
-        <v>59</v>
-      </c>
-      <c r="C16">
-        <v>22</v>
-      </c>
-      <c r="D16">
-        <v>291</v>
-      </c>
-      <c r="E16">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17">
-        <v>59</v>
-      </c>
-      <c r="C17">
-        <v>22</v>
-      </c>
-      <c r="D17">
-        <v>224</v>
-      </c>
-      <c r="E17">
-        <v>258</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B18">
         <v>59</v>
@@ -624,15 +630,15 @@
         <v>22</v>
       </c>
       <c r="D18">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="E18">
-        <v>258</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B19">
         <v>59</v>
@@ -641,13 +647,48 @@
         <v>22</v>
       </c>
       <c r="D19">
-        <v>363</v>
+        <v>223</v>
       </c>
       <c r="E19">
-        <v>258</v>
+        <v>247</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20">
+        <v>59</v>
+      </c>
+      <c r="C20">
+        <v>22</v>
+      </c>
+      <c r="D20">
+        <v>288</v>
+      </c>
+      <c r="E20">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21">
+        <v>59</v>
+      </c>
+      <c r="C21">
+        <v>22</v>
+      </c>
+      <c r="D21">
+        <v>355</v>
+      </c>
+      <c r="E21">
+        <v>247</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>